<commit_message>
Recoding of study codes so that they alphabeticise correctly (discovery that one study had first and second author order swapped led to updated .bib file but without update of study codes, was being represented in wrong order. In addition, finding of mistyping of sample size (52 rather than 32) now corrected
</commit_message>
<xml_diff>
--- a/data/study_overview_sheet.xlsx
+++ b/data/study_overview_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2509920f_student_gla_ac_uk/Documents/DClin/Deliverables/Systematic Review/Writeup/DCLIN_SR_git/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/alexander_fradera_glasgow_ac_uk/Documents/Documents/2. Research/1. Ongoing research/pre-qualification research projects/DCLIN_SR_git/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3397" documentId="8_{7F86DA56-8D65-4C4F-B68E-F6A80F78D27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C467A6A3-E617-4887-8964-8DDA923F3ECC}"/>
+  <xr:revisionPtr revIDLastSave="3403" documentId="8_{7F86DA56-8D65-4C4F-B68E-F6A80F78D27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A62F85C-01FB-411E-ABB4-32AEDD37F371}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="1110" windowWidth="28770" windowHeight="16890" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="742" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study_overview" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="346">
   <si>
     <t>Pain Medicine</t>
   </si>
@@ -521,9 +521,6 @@
     <t>BAR026</t>
   </si>
   <si>
-    <t>BOL034</t>
-  </si>
-  <si>
     <t>BOR37</t>
   </si>
   <si>
@@ -1071,6 +1068,15 @@
   </si>
   <si>
     <t>Australia</t>
+  </si>
+  <si>
+    <t>ethno_racial</t>
+  </si>
+  <si>
+    <t>not reported</t>
+  </si>
+  <si>
+    <t>RAT034</t>
   </si>
 </sst>
 </file>
@@ -1123,27 +1129,27 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1435,10 +1441,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B9E2A3-88A1-47CD-91E6-035C20FAA1A2}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,21 +1466,21 @@
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>248</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>1</v>
@@ -1483,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>4</v>
@@ -1491,10 +1500,13 @@
       <c r="K1" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" s="1">
         <v>9</v>
@@ -1506,7 +1518,7 @@
         <v>44624</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -1515,7 +1527,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>10</v>
@@ -1527,9 +1539,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3" s="1">
         <v>16</v>
@@ -1541,7 +1553,7 @@
         <v>44624</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>13</v>
@@ -1550,7 +1562,7 @@
         <v>49</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>125</v>
@@ -1562,9 +1574,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B4" s="1">
         <v>26</v>
@@ -1576,7 +1588,7 @@
         <v>44624</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -1585,7 +1597,7 @@
         <v>50</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>126</v>
@@ -1597,21 +1609,21 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B5" s="1">
         <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>160</v>
+        <v>345</v>
       </c>
       <c r="D5" s="2">
         <v>44624</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>15</v>
@@ -1620,7 +1632,7 @@
         <v>51</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>127</v>
@@ -1632,21 +1644,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B6" s="1">
         <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="2">
         <v>44632</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>16</v>
@@ -1655,7 +1667,7 @@
         <v>52</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>128</v>
@@ -1667,21 +1679,21 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B7" s="1">
         <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="2">
         <v>44632</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>17</v>
@@ -1690,7 +1702,7 @@
         <v>53</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>129</v>
@@ -1702,21 +1714,21 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B8" s="1">
         <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D8" s="2">
         <v>44632</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>18</v>
@@ -1725,7 +1737,7 @@
         <v>54</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>130</v>
@@ -1737,56 +1749,56 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B9" s="1">
         <v>194</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D9" s="2">
         <v>44326</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10" s="1">
         <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D10" s="2">
         <v>44632</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>19</v>
@@ -1795,7 +1807,7 @@
         <v>55</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>126</v>
@@ -1807,30 +1819,30 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B11" s="1">
         <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D11" s="2">
         <v>44632</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>341</v>
-      </c>
       <c r="H11" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
@@ -1840,21 +1852,21 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B12" s="1">
         <v>69</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D12" s="2">
         <v>44632</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>20</v>
@@ -1863,7 +1875,7 @@
         <v>56</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>126</v>
@@ -1875,21 +1887,21 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B13" s="1">
         <v>70</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D13" s="2">
         <v>44632</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>21</v>
@@ -1898,7 +1910,7 @@
         <v>57</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>131</v>
@@ -1910,21 +1922,21 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B14" s="1">
         <v>77</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D14" s="2">
         <v>44633</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>22</v>
@@ -1933,7 +1945,7 @@
         <v>58</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>132</v>
@@ -1945,21 +1957,21 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B15" s="1">
         <v>79</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D15" s="2">
         <v>44633</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>23</v>
@@ -1968,7 +1980,7 @@
         <v>59</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>133</v>
@@ -1980,21 +1992,21 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B16" s="1">
         <v>83</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D16" s="2">
         <v>44633</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>24</v>
@@ -2003,7 +2015,7 @@
         <v>60</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>134</v>
@@ -2017,19 +2029,19 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B17" s="1">
         <v>89</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D17" s="2">
         <v>44633</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>25</v>
@@ -2038,7 +2050,7 @@
         <v>61</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>135</v>
@@ -2052,19 +2064,19 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B18" s="1">
         <v>90</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D18" s="2">
         <v>44633</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>26</v>
@@ -2073,7 +2085,7 @@
         <v>62</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>126</v>
@@ -2087,19 +2099,19 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B19" s="1">
         <v>92</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D19" s="2">
         <v>44633</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>27</v>
@@ -2108,7 +2120,7 @@
         <v>63</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>136</v>
@@ -2122,19 +2134,19 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B20" s="1">
         <v>95</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D20" s="2">
         <v>44633</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>28</v>
@@ -2143,7 +2155,7 @@
         <v>64</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>137</v>
@@ -2157,19 +2169,19 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B21" s="1">
         <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" s="2">
         <v>44633</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>29</v>
@@ -2178,7 +2190,7 @@
         <v>65</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>138</v>
@@ -2192,19 +2204,19 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B22" s="1">
         <v>102</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D22" s="2">
         <v>44633</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>30</v>
@@ -2213,7 +2225,7 @@
         <v>66</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>139</v>
@@ -2227,19 +2239,19 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B23" s="1">
         <v>103</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D23" s="2">
         <v>44633</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>31</v>
@@ -2248,7 +2260,7 @@
         <v>67</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>140</v>
@@ -2262,19 +2274,19 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B24" s="1">
         <v>113</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D24" s="2">
         <v>44633</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>32</v>
@@ -2283,7 +2295,7 @@
         <v>68</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>141</v>
@@ -2297,19 +2309,19 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B25" s="1">
         <v>114</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D25" s="2">
         <v>44633</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>33</v>
@@ -2318,7 +2330,7 @@
         <v>69</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>142</v>
@@ -2332,19 +2344,19 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B26" s="1">
         <v>120</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D26" s="2">
         <v>44633</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>34</v>
@@ -2353,7 +2365,7 @@
         <v>70</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>143</v>
@@ -2367,19 +2379,19 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B27" s="1">
         <v>121</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D27" s="2">
         <v>44633</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>35</v>
@@ -2388,7 +2400,7 @@
         <v>71</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>144</v>
@@ -2402,19 +2414,19 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B28" s="1">
         <v>125</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D28" s="2">
         <v>44633</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>36</v>
@@ -2423,7 +2435,7 @@
         <v>72</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>145</v>
@@ -2437,32 +2449,32 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B29" s="3">
         <v>128</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D29" s="1">
         <v>44652</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F29" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="G29" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>238</v>
-      </c>
       <c r="H29" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>112</v>
@@ -2470,34 +2482,34 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B30" s="1">
         <v>134</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D30" s="2">
         <v>44647</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>115</v>
@@ -2505,19 +2517,19 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B31" s="1">
         <v>136</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D31" s="2">
         <v>44647</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>37</v>
@@ -2526,7 +2538,7 @@
         <v>73</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>146</v>
@@ -2540,19 +2552,19 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B32" s="1">
         <v>137</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D32" s="2">
         <v>44647</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>38</v>
@@ -2561,7 +2573,7 @@
         <v>74</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>147</v>
@@ -2575,19 +2587,19 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B33" s="1">
         <v>143</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D33" s="2">
         <v>44647</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>39</v>
@@ -2596,7 +2608,7 @@
         <v>75</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>148</v>
@@ -2610,19 +2622,19 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B34" s="1">
         <v>144</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D34" s="2">
         <v>44647</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>40</v>
@@ -2631,7 +2643,7 @@
         <v>76</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>149</v>
@@ -2645,19 +2657,19 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B35" s="1">
         <v>149</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D35" s="2">
         <v>44674</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>41</v>
@@ -2666,7 +2678,7 @@
         <v>77</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>150</v>
@@ -2680,32 +2692,32 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B36" s="1">
         <v>999</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D36" s="2">
         <v>44326</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K36" s="1">
         <v>2015</v>
@@ -2713,19 +2725,19 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B37" s="1">
         <v>156</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D37" s="2">
         <v>44674</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>42</v>
@@ -2734,7 +2746,7 @@
         <v>78</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>151</v>
@@ -2748,34 +2760,34 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B38" s="1">
         <v>158</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D38" s="2">
         <v>44674</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>113</v>
@@ -2783,19 +2795,19 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B39" s="1">
         <v>167</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D39" s="2">
         <v>44674</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>43</v>
@@ -2804,7 +2816,7 @@
         <v>79</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>152</v>
@@ -2818,19 +2830,19 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B40" s="1">
         <v>171</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D40" s="2">
         <v>44674</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>44</v>
@@ -2839,7 +2851,7 @@
         <v>80</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>153</v>
@@ -2853,19 +2865,19 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B41" s="1">
         <v>173</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D41" s="2">
         <v>44674</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>45</v>
@@ -2874,7 +2886,7 @@
         <v>81</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>154</v>
@@ -2888,19 +2900,19 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B42" s="1">
         <v>178</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D42" s="2">
         <v>44674</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>46</v>
@@ -2909,7 +2921,7 @@
         <v>82</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>155</v>
@@ -2923,28 +2935,28 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B43" s="1">
         <v>182</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D43" s="2">
         <v>44674</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1" t="s">
@@ -2956,19 +2968,19 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B44" s="1">
         <v>183</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D44" s="2">
         <v>44674</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>47</v>
@@ -2977,7 +2989,7 @@
         <v>83</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>156</v>
@@ -2991,19 +3003,19 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B45" s="1">
         <v>184</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D45" s="2">
         <v>44674</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>48</v>
@@ -3012,7 +3024,7 @@
         <v>5</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>157</v>
@@ -3026,28 +3038,28 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B46" s="3">
         <v>186</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F46" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G46" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="H46" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="J46" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>244</v>
       </c>
       <c r="K46" s="3" t="s">
         <v>112</v>
@@ -3055,31 +3067,31 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B47" s="3">
         <v>998</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D47" s="9">
         <v>44716</v>
       </c>
       <c r="E47" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="G47" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="H47" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="J47" s="3" t="s">
         <v>296</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>297</v>
       </c>
       <c r="K47" s="4">
         <v>2010</v>
@@ -3087,234 +3099,237 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B48" s="3">
         <v>991</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K48" s="4">
         <v>2020</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B49" s="3">
         <v>992</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K49" s="4">
         <v>2017</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B50" s="3">
         <v>197</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F50" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="G50" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="G50" s="3" t="s">
-        <v>308</v>
-      </c>
       <c r="H50" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K50" s="4">
         <v>2019</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B51" s="3">
         <v>994</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K51" s="4">
         <v>2018</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B52" s="3">
         <v>995</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F52" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="G52" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="G52" s="3" t="s">
-        <v>312</v>
-      </c>
       <c r="H52" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J52" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K52" s="4">
         <v>2012</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B53" s="3">
         <v>196</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K53" s="4">
         <v>2012</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B54" s="3">
         <v>997</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K54" s="4">
         <v>2012</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B55" s="3">
         <v>195</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="I55" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="I55" s="3" t="s">
+      <c r="J55" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="J55" s="3" t="s">
-        <v>337</v>
       </c>
       <c r="K55" s="4">
         <v>2021</v>

</xml_diff>